<commit_message>
Update BattGO AT Command Communication Protocol_1.3.xlsx
</commit_message>
<xml_diff>
--- a/Media/BattGO AT Command Communication Protocol_1.3.xlsx
+++ b/Media/BattGO AT Command Communication Protocol_1.3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23263" windowHeight="13183" tabRatio="220"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="220"/>
   </bookViews>
   <sheets>
     <sheet name="BattGO AT Command Communication" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="261">
   <si>
     <t>BattGO AT Command Communication Protocol</t>
   </si>
@@ -290,9 +290,6 @@
     <t>UVC</t>
   </si>
   <si>
-    <t>For example, query 6S battery cell voltage per cell:</t>
-  </si>
-  <si>
     <t>Cell start number (starting from 0, ASCII characters)</t>
   </si>
   <si>
@@ -870,17 +867,17 @@
     <t>%&lt;COMMAND&gt; &lt;DATA&gt;&lt;LF&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">25 55 50 43 20 31 20 30 30 30 30 30 64 31 36 20 30 65 64 38 20 31 30 36 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">38 20 33 63 0A </t>
+    <t>For example, query 4S battery cell voltage per cell:</t>
+  </si>
+  <si>
+    <t>&amp;UVC 1 0 3\n</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1029,6 +1026,13 @@
       <color theme="0"/>
       <name val="微软雅黑"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1247,7 +1251,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1456,15 +1460,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1474,29 +1505,56 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1507,9 +1565,6 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1518,54 +1573,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1651,6 +1658,120 @@
         <a:xfrm>
           <a:off x="161925" y="36937950"/>
           <a:ext cx="6164580" cy="4088765"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>665018</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>141316</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3906764</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>58170</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Immagine 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9767454" y="26858421"/>
+          <a:ext cx="3241746" cy="282614"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>216131</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>24938</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4031416</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>83111</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Immagine 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9318567" y="16168254"/>
+          <a:ext cx="3815285" cy="241053"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>265666</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>149594</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Immagine 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9102436" y="32028938"/>
+          <a:ext cx="5078735" cy="515354"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2032,11 +2153,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H159"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="57" style="32" customWidth="1"/>
     <col min="2" max="2" width="64.6640625" style="32" customWidth="1"/>
@@ -2045,10 +2166,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="83"/>
+      <c r="B3" s="78"/>
     </row>
     <row r="4" spans="1:3">
       <c r="C4" s="33" t="s">
@@ -2075,7 +2196,7 @@
       <c r="A7" s="36"/>
       <c r="B7" s="38"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" ht="15.6">
       <c r="A8" s="39" t="s">
         <v>4</v>
       </c>
@@ -2236,16 +2357,16 @@
       <c r="B29" s="49"/>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="84" t="s">
+      <c r="A31" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="85"/>
+      <c r="B31" s="80"/>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="50" t="s">
+      <c r="B32" s="72" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2268,7 +2389,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="24.9">
+    <row r="35" spans="1:3" ht="26.4">
       <c r="A35" s="53" t="s">
         <v>36</v>
       </c>
@@ -2283,7 +2404,7 @@
       <c r="A38" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="50" t="s">
+      <c r="B38" s="72" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2306,7 +2427,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" ht="14.4">
       <c r="A41" s="53" t="s">
         <v>36</v>
       </c>
@@ -2317,7 +2438,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="26.2">
+    <row r="44" spans="1:3" ht="26.4">
       <c r="A44" s="50" t="s">
         <v>44</v>
       </c>
@@ -2345,7 +2466,7 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="75" t="s">
+      <c r="A47" s="84" t="s">
         <v>36</v>
       </c>
       <c r="B47" s="57" t="s">
@@ -2356,16 +2477,16 @@
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="76"/>
+      <c r="A48" s="85"/>
       <c r="B48" s="57" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="74" t="s">
+      <c r="A51" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="74"/>
+      <c r="B51" s="81"/>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="50" t="s">
@@ -2394,8 +2515,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="24.9">
-      <c r="A56" s="75" t="s">
+    <row r="56" spans="1:4" ht="26.4">
+      <c r="A56" s="84" t="s">
         <v>36</v>
       </c>
       <c r="B56" s="58" t="s">
@@ -2403,14 +2524,14 @@
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="76"/>
+      <c r="A57" s="85"/>
       <c r="B57" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="C57" s="72" t="s">
+      <c r="C57" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="D57" s="73"/>
+      <c r="D57" s="83"/>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="59"/>
@@ -2448,7 +2569,7 @@
       </c>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="75" t="s">
+      <c r="A63" s="84" t="s">
         <v>36</v>
       </c>
       <c r="B63" s="56" t="s">
@@ -2456,7 +2577,7 @@
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="76"/>
+      <c r="A64" s="85"/>
       <c r="B64" s="56" t="s">
         <v>62</v>
       </c>
@@ -2465,19 +2586,19 @@
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="76"/>
+      <c r="A65" s="85"/>
       <c r="B65" s="56" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="76"/>
+      <c r="A66" s="85"/>
       <c r="B66" s="56" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="76"/>
+      <c r="A67" s="85"/>
       <c r="B67" s="56" t="s">
         <v>66</v>
       </c>
@@ -2494,7 +2615,7 @@
       <c r="A70" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="B70" s="50" t="s">
+      <c r="B70" s="72" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2516,23 +2637,19 @@
       <c r="C72" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="D72" s="63" t="s">
-        <v>260</v>
-      </c>
+      <c r="D72" s="63"/>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="75" t="s">
+      <c r="A73" s="84" t="s">
         <v>36</v>
       </c>
       <c r="B73" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="D73" s="63" t="s">
-        <v>261</v>
-      </c>
+      <c r="D73" s="63"/>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="76"/>
+      <c r="A74" s="85"/>
       <c r="B74" s="56" t="s">
         <v>70</v>
       </c>
@@ -2541,19 +2658,19 @@
       </c>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="76"/>
+      <c r="A75" s="85"/>
       <c r="B75" s="56" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="76"/>
+      <c r="A76" s="85"/>
       <c r="B76" s="56" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="76"/>
+      <c r="A77" s="85"/>
       <c r="B77" s="56" t="s">
         <v>74</v>
       </c>
@@ -2570,7 +2687,7 @@
       <c r="A80" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="B80" s="50" t="s">
+      <c r="B80" s="72" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2583,74 +2700,74 @@
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="77" t="s">
+      <c r="A82" s="86" t="s">
         <v>34</v>
       </c>
       <c r="B82" s="55" t="s">
         <v>53</v>
       </c>
       <c r="C82" s="33" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="86"/>
+      <c r="B83" s="55" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="77"/>
-      <c r="B83" s="55" t="s">
-        <v>78</v>
-      </c>
       <c r="C83" s="33" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="86"/>
+      <c r="B84" s="55" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="77"/>
-      <c r="B84" s="55" t="s">
-        <v>80</v>
-      </c>
-    </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="75" t="s">
+      <c r="A85" s="84" t="s">
         <v>36</v>
       </c>
       <c r="B85" s="58" t="s">
         <v>61</v>
       </c>
       <c r="C85" s="33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="85"/>
+      <c r="B86" s="56" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="76"/>
-      <c r="B86" s="56" t="s">
+    <row r="87" spans="1:3">
+      <c r="A87" s="85"/>
+      <c r="B87" s="56" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="76"/>
-      <c r="B87" s="56" t="s">
+    <row r="88" spans="1:3">
+      <c r="A88" s="85"/>
+      <c r="B88" s="56" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="76"/>
-      <c r="B88" s="56" t="s">
+    <row r="89" spans="1:3">
+      <c r="A89" s="85"/>
+      <c r="B89" s="56" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="76"/>
-      <c r="B89" s="56" t="s">
+    <row r="90" spans="1:3">
+      <c r="A90" s="85"/>
+      <c r="B90" s="56" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="76"/>
-      <c r="B90" s="56" t="s">
-        <v>86</v>
-      </c>
-    </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="76"/>
+      <c r="A91" s="85"/>
       <c r="B91" s="56" t="s">
         <v>70</v>
       </c>
@@ -2665,10 +2782,10 @@
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="B94" s="50" t="s">
         <v>87</v>
-      </c>
-      <c r="B94" s="50" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2680,7 +2797,7 @@
       </c>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="77" t="s">
+      <c r="A96" s="86" t="s">
         <v>34</v>
       </c>
       <c r="B96" s="55" t="s">
@@ -2688,47 +2805,47 @@
       </c>
     </row>
     <row r="97" spans="1:6">
-      <c r="A97" s="77"/>
+      <c r="A97" s="86"/>
       <c r="B97" s="55" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="86"/>
+      <c r="B98" s="55" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="98" spans="1:6">
-      <c r="A98" s="77"/>
-      <c r="B98" s="55" t="s">
+      <c r="C98" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="C98" s="33" t="s">
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" s="86"/>
+      <c r="B99" s="55" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
-      <c r="A99" s="77"/>
-      <c r="B99" s="55" t="s">
+    <row r="100" spans="1:6">
+      <c r="A100" s="86"/>
+      <c r="B100" s="55" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
-      <c r="A100" s="77"/>
-      <c r="B100" s="55" t="s">
-        <v>93</v>
-      </c>
-    </row>
     <row r="101" spans="1:6">
-      <c r="A101" s="75" t="s">
+      <c r="A101" s="84" t="s">
         <v>36</v>
       </c>
       <c r="B101" s="56" t="s">
         <v>61</v>
       </c>
       <c r="C101" s="33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" s="85"/>
+      <c r="B102" s="56" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
-      <c r="A102" s="76"/>
-      <c r="B102" s="56" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2741,10 +2858,10 @@
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="B105" s="50" t="s">
         <v>96</v>
-      </c>
-      <c r="B105" s="50" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -2755,62 +2872,62 @@
         <v>24</v>
       </c>
       <c r="C106" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="107" spans="1:6">
-      <c r="A107" s="77" t="s">
+      <c r="A107" s="86" t="s">
         <v>34</v>
       </c>
       <c r="B107" s="55" t="s">
         <v>53</v>
       </c>
       <c r="C107" s="33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" s="86"/>
+      <c r="B108" s="55" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
-      <c r="A108" s="77"/>
-      <c r="B108" s="55" t="s">
-        <v>100</v>
-      </c>
-    </row>
     <row r="109" spans="1:6">
-      <c r="A109" s="75" t="s">
+      <c r="A109" s="84" t="s">
         <v>36</v>
       </c>
       <c r="B109" s="56" t="s">
         <v>61</v>
       </c>
       <c r="C109" s="33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" s="85"/>
+      <c r="B110" s="56" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="110" spans="1:6">
-      <c r="A110" s="76"/>
-      <c r="B110" s="56" t="s">
+      <c r="C110" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="C110" s="33" t="s">
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" s="85"/>
+      <c r="B111" s="56" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="111" spans="1:6">
-      <c r="A111" s="76"/>
-      <c r="B111" s="56" t="s">
+      <c r="C111" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="C111" s="33" t="s">
+    </row>
+    <row r="112" spans="1:6" ht="144">
+      <c r="A112" s="85"/>
+      <c r="B112" s="56" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" ht="130.94999999999999">
-      <c r="A112" s="76"/>
-      <c r="B112" s="56" t="s">
+      <c r="C112" s="60" t="s">
         <v>106</v>
-      </c>
-      <c r="C112" s="60" t="s">
-        <v>107</v>
       </c>
       <c r="D112" s="61"/>
       <c r="E112" s="61"/>
@@ -2818,10 +2935,10 @@
     </row>
     <row r="116" spans="1:8">
       <c r="A116" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="B116" s="50" t="s">
         <v>108</v>
-      </c>
-      <c r="B116" s="50" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -2840,71 +2957,71 @@
         <v>53</v>
       </c>
       <c r="C118" s="33" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="26.4">
+      <c r="A119" s="84" t="s">
+        <v>36</v>
+      </c>
+      <c r="B119" s="54" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="24.9">
-      <c r="A119" s="75" t="s">
-        <v>36</v>
-      </c>
-      <c r="B119" s="54" t="s">
+    <row r="120" spans="1:8">
+      <c r="A120" s="85"/>
+      <c r="B120" s="57" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="120" spans="1:8">
-      <c r="A120" s="76"/>
-      <c r="B120" s="57" t="s">
+      <c r="C120" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="C120" s="33" t="s">
+    </row>
+    <row r="121" spans="1:8">
+      <c r="A121" s="85"/>
+      <c r="B121" s="57" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
-      <c r="A121" s="76"/>
-      <c r="B121" s="57" t="s">
+    <row r="122" spans="1:8">
+      <c r="A122" s="85"/>
+      <c r="B122" s="57" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
-      <c r="A122" s="76"/>
-      <c r="B122" s="57" t="s">
+    <row r="123" spans="1:8">
+      <c r="A123" s="85"/>
+      <c r="B123" s="57" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
-      <c r="A123" s="76"/>
-      <c r="B123" s="57" t="s">
+    <row r="124" spans="1:8">
+      <c r="A124" s="85"/>
+      <c r="B124" s="57" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
-      <c r="A124" s="76"/>
-      <c r="B124" s="57" t="s">
+    <row r="125" spans="1:8">
+      <c r="A125" s="85"/>
+      <c r="B125" s="57" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="125" spans="1:8">
-      <c r="A125" s="76"/>
-      <c r="B125" s="57" t="s">
+      <c r="H125" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="H125" s="63" t="s">
+    </row>
+    <row r="128" spans="1:8" ht="15.6">
+      <c r="A128" s="81" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="128" spans="1:8">
-      <c r="A128" s="74" t="s">
-        <v>120</v>
-      </c>
-      <c r="B128" s="74"/>
+      <c r="B128" s="81"/>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="B129" s="50" t="s">
         <v>121</v>
-      </c>
-      <c r="B129" s="50" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2923,68 +3040,68 @@
         <v>53</v>
       </c>
       <c r="C131" s="33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="132" spans="1:4">
-      <c r="A132" s="78" t="s">
+      <c r="A132" s="73" t="s">
         <v>36</v>
       </c>
       <c r="B132" s="55" t="s">
         <v>61</v>
       </c>
+      <c r="C132" s="33" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="133" spans="1:4">
-      <c r="A133" s="79"/>
+      <c r="A133" s="74"/>
       <c r="B133" s="57" t="s">
-        <v>124</v>
-      </c>
-      <c r="C133" s="33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="74"/>
+      <c r="B134" s="57" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
-      <c r="A134" s="79"/>
-      <c r="B134" s="57" t="s">
+    <row r="135" spans="1:4">
+      <c r="A135" s="74"/>
+      <c r="B135" s="57" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
-      <c r="A135" s="79"/>
-      <c r="B135" s="57" t="s">
+    <row r="136" spans="1:4">
+      <c r="A136" s="74"/>
+      <c r="B136" s="57" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
-      <c r="A136" s="79"/>
-      <c r="B136" s="57" t="s">
+    <row r="137" spans="1:4">
+      <c r="A137" s="75"/>
+      <c r="B137" s="57" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4">
-      <c r="A137" s="80"/>
-      <c r="B137" s="57" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="64"/>
       <c r="B138" s="65"/>
     </row>
-    <row r="139" spans="1:4" ht="87.05">
+    <row r="139" spans="1:4" ht="92.4">
       <c r="A139" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="B139" s="67" t="s">
         <v>130</v>
-      </c>
-      <c r="B139" s="67" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="B142" s="69" t="s">
         <v>132</v>
-      </c>
-      <c r="B142" s="69" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -3003,14 +3120,14 @@
         <v>53</v>
       </c>
       <c r="C144" s="33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D144" s="34" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="145" spans="1:5">
-      <c r="A145" s="81" t="s">
+      <c r="A145" s="76" t="s">
         <v>36</v>
       </c>
       <c r="B145" s="57" t="s">
@@ -3021,138 +3138,138 @@
       </c>
     </row>
     <row r="146" spans="1:5">
-      <c r="A146" s="82"/>
+      <c r="A146" s="77"/>
       <c r="B146" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="C146" s="33" t="s">
         <v>135</v>
-      </c>
-      <c r="C146" s="33" t="s">
-        <v>136</v>
       </c>
       <c r="E146" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:5">
-      <c r="A147" s="82"/>
+      <c r="A147" s="77"/>
       <c r="B147" s="57" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E147" s="34">
         <v>2</v>
       </c>
     </row>
     <row r="148" spans="1:5">
-      <c r="A148" s="82"/>
+      <c r="A148" s="77"/>
       <c r="B148" s="57" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E148" s="34">
         <v>2</v>
       </c>
     </row>
     <row r="149" spans="1:5">
-      <c r="A149" s="82"/>
+      <c r="A149" s="77"/>
       <c r="B149" s="57" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E149" s="34">
         <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:5">
-      <c r="A150" s="82"/>
+      <c r="A150" s="77"/>
       <c r="B150" s="57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E150" s="34">
         <v>2</v>
       </c>
     </row>
     <row r="151" spans="1:5">
-      <c r="A151" s="82"/>
+      <c r="A151" s="77"/>
       <c r="B151" s="57" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E151" s="34">
         <v>4</v>
       </c>
     </row>
     <row r="152" spans="1:5">
-      <c r="A152" s="82"/>
+      <c r="A152" s="77"/>
       <c r="B152" s="57" t="s">
+        <v>141</v>
+      </c>
+      <c r="C152" s="33" t="s">
         <v>142</v>
-      </c>
-      <c r="C152" s="33" t="s">
-        <v>143</v>
       </c>
       <c r="E152" s="34">
         <v>2</v>
       </c>
     </row>
     <row r="153" spans="1:5">
-      <c r="A153" s="82"/>
+      <c r="A153" s="77"/>
       <c r="B153" s="57" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C153" s="33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E153" s="34">
         <v>2</v>
       </c>
     </row>
     <row r="154" spans="1:5">
-      <c r="A154" s="82"/>
+      <c r="A154" s="77"/>
       <c r="B154" s="57" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E154" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:5">
-      <c r="A155" s="82"/>
+      <c r="A155" s="77"/>
       <c r="B155" s="57" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E155" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:5">
-      <c r="A156" s="82"/>
+      <c r="A156" s="77"/>
       <c r="B156" s="57" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E156" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:5">
-      <c r="A157" s="82"/>
+      <c r="A157" s="77"/>
       <c r="B157" s="57" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E157" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:5">
-      <c r="A158" s="82"/>
+      <c r="A158" s="77"/>
       <c r="B158" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="C158" s="33" t="s">
         <v>148</v>
-      </c>
-      <c r="C158" s="33" t="s">
-        <v>149</v>
       </c>
       <c r="E158" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:5">
-      <c r="A159" s="82"/>
+      <c r="A159" s="77"/>
       <c r="B159" s="57" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E159" s="34">
         <v>1</v>
@@ -3160,11 +3277,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A132:A137"/>
-    <mergeCell ref="A145:A159"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A51:B51"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="A128:B128"/>
     <mergeCell ref="A47:A48"/>
@@ -3178,10 +3290,15 @@
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="A109:A112"/>
     <mergeCell ref="A119:A125"/>
+    <mergeCell ref="A132:A137"/>
+    <mergeCell ref="A145:A159"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A51:B51"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3193,7 +3310,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
@@ -3201,10 +3318,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="71" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1" s="71" t="s">
         <v>258</v>
-      </c>
-      <c r="C1" s="71" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3226,143 +3343,143 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="37.109375" customWidth="1"/>
     <col min="2" max="2" width="51.21875" customWidth="1"/>
     <col min="3" max="3" width="32.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:3" ht="19.649999999999999">
+    <row r="4" spans="1:3" ht="20.399999999999999">
       <c r="A4" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.6">
+      <c r="A5" s="4" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16.399999999999999">
-      <c r="A5" s="4" t="s">
-        <v>153</v>
       </c>
       <c r="B5" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.399999999999999">
+    <row r="6" spans="1:3" ht="15.6">
       <c r="A6" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B6" s="6">
         <v>42971</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.399999999999999">
+    <row r="7" spans="1:3" ht="15.6">
       <c r="A7" s="4"/>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:3" ht="17.05">
+    <row r="8" spans="1:3" ht="16.2">
       <c r="A8" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B8" s="8" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="16.2">
+      <c r="A9" s="9" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17.05">
-      <c r="A9" s="9" t="s">
-        <v>157</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.05">
+    <row r="10" spans="1:3" ht="16.2">
       <c r="A10" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.05">
+    <row r="11" spans="1:3" ht="16.2">
       <c r="A11" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17.05">
+    <row r="12" spans="1:3" ht="16.2">
       <c r="A12" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.05">
+    <row r="13" spans="1:3" ht="16.2">
       <c r="A13" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="B13" s="10" t="s">
+    </row>
+    <row r="14" spans="1:3" ht="16.2">
+      <c r="A14" s="9" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="17.05">
-      <c r="A14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>163</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="11"/>
       <c r="B15" s="12"/>
     </row>
-    <row r="16" spans="1:3" ht="17.05">
+    <row r="16" spans="1:3" ht="16.2">
       <c r="A16" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B16" s="7"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="B17" s="8" t="s">
+    </row>
+    <row r="18" spans="1:2" ht="16.2">
+      <c r="A18" s="14" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="17.05">
-      <c r="A18" s="14" t="s">
-        <v>168</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17.05">
+    <row r="19" spans="1:2" ht="16.2">
       <c r="A19" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="B19" s="15" t="s">
+    </row>
+    <row r="20" spans="1:2" ht="16.2">
+      <c r="A20" s="14" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="17.05">
-      <c r="A20" s="14" t="s">
+      <c r="B20" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="B20" s="15" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="16.2">
+      <c r="A21" s="14" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="17.05">
-      <c r="A21" s="14" t="s">
-        <v>173</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>27</v>
@@ -3374,299 +3491,299 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B23" s="12"/>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="B24" s="8" t="s">
+    </row>
+    <row r="25" spans="1:2" ht="16.2">
+      <c r="A25" s="14" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="17.05">
-      <c r="A25" s="14" t="s">
-        <v>168</v>
       </c>
       <c r="B25" s="70" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="17.05">
+    <row r="26" spans="1:2" ht="16.2">
       <c r="A26" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B26" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="B26" s="15" t="s">
+    </row>
+    <row r="27" spans="1:2" ht="16.2">
+      <c r="A27" s="14" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="17.05">
-      <c r="A27" s="14" t="s">
+      <c r="B27" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="B27" s="15" t="s">
+    </row>
+    <row r="28" spans="1:2" ht="16.2">
+      <c r="A28" s="14" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="17.05">
-      <c r="A28" s="14" t="s">
-        <v>173</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="17.05">
+    <row r="29" spans="1:2" ht="16.2">
       <c r="A29" s="17"/>
       <c r="B29" s="18"/>
     </row>
-    <row r="31" spans="1:2" ht="17.05">
-      <c r="A31" s="86" t="s">
+    <row r="31" spans="1:2" ht="16.2">
+      <c r="A31" s="104" t="s">
+        <v>174</v>
+      </c>
+      <c r="B31" s="105"/>
+    </row>
+    <row r="32" spans="1:2" ht="16.2">
+      <c r="A32" s="19" t="s">
         <v>175</v>
-      </c>
-      <c r="B31" s="87"/>
-    </row>
-    <row r="32" spans="1:2" ht="17.05">
-      <c r="A32" s="19" t="s">
-        <v>176</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17.05">
+    <row r="33" spans="1:3" ht="16.2">
       <c r="A33" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="17.05">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="16.2">
       <c r="A34" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="17.05">
+    <row r="35" spans="1:3" ht="31.2">
       <c r="A35" s="22" t="s">
         <v>36</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="17.05">
+    <row r="38" spans="1:3" ht="16.2">
       <c r="A38" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B38" s="19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="17.05">
+    <row r="39" spans="1:3" ht="16.2">
       <c r="A39" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="17.05">
+    <row r="40" spans="1:3" ht="16.2">
       <c r="A40" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="17.05">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="16.2">
       <c r="A41" s="22" t="s">
         <v>36</v>
       </c>
       <c r="B41" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C41" s="1" t="s">
+    </row>
+    <row r="44" spans="1:3" ht="16.2">
+      <c r="A44" s="19" t="s">
         <v>181</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="17.05">
-      <c r="A44" s="19" t="s">
-        <v>182</v>
       </c>
       <c r="B44" s="19" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="17.05">
+    <row r="45" spans="1:3" ht="16.2">
       <c r="A45" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="17.05">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="16.2">
       <c r="A46" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="16.399999999999999">
-      <c r="A47" s="90" t="s">
+    <row r="47" spans="1:3" ht="15.6">
+      <c r="A47" s="107" t="s">
         <v>36</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="16.399999999999999">
-      <c r="A48" s="91"/>
+    <row r="48" spans="1:3" ht="15.6">
+      <c r="A48" s="108"/>
       <c r="B48" s="26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="16.2">
+      <c r="A51" s="106" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="17.05">
-      <c r="A51" s="88" t="s">
+      <c r="B51" s="106"/>
+    </row>
+    <row r="53" spans="1:4" ht="16.2">
+      <c r="A53" s="19" t="s">
         <v>185</v>
-      </c>
-      <c r="B51" s="88"/>
-    </row>
-    <row r="53" spans="1:4" ht="17.05">
-      <c r="A53" s="19" t="s">
-        <v>186</v>
       </c>
       <c r="B53" s="19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="17.05">
+    <row r="54" spans="1:4" ht="16.2">
       <c r="A54" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="17.05">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="16.2">
       <c r="A55" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="16.399999999999999">
-      <c r="A56" s="90" t="s">
+    <row r="56" spans="1:4" ht="15.6">
+      <c r="A56" s="107" t="s">
         <v>36</v>
       </c>
       <c r="B56" s="25" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.6">
+      <c r="A57" s="108"/>
+      <c r="B57" s="26" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="16.399999999999999">
-      <c r="A57" s="91"/>
-      <c r="B57" s="26" t="s">
-        <v>189</v>
-      </c>
-      <c r="C57" s="89" t="s">
+      <c r="C57" s="90" t="s">
         <v>57</v>
       </c>
-      <c r="D57" s="89"/>
-    </row>
-    <row r="58" spans="1:4" ht="17.05">
+      <c r="D57" s="90"/>
+    </row>
+    <row r="58" spans="1:4" ht="16.2">
       <c r="A58" s="27"/>
       <c r="B58" s="27"/>
     </row>
-    <row r="59" spans="1:4" ht="17.05">
+    <row r="59" spans="1:4" ht="16.2">
       <c r="A59" s="27"/>
       <c r="B59" s="27"/>
     </row>
-    <row r="60" spans="1:4" ht="17.05">
+    <row r="60" spans="1:4" ht="16.2">
       <c r="A60" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B60" s="19" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="17.05">
+    <row r="61" spans="1:4" ht="16.2">
       <c r="A61" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="17.05">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="16.2">
       <c r="A62" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="16.399999999999999">
-      <c r="A63" s="90" t="s">
+    <row r="63" spans="1:4" ht="15.6">
+      <c r="A63" s="107" t="s">
         <v>36</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="16.399999999999999">
-      <c r="A64" s="91"/>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15.6">
+      <c r="A64" s="108"/>
       <c r="B64" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="16.399999999999999">
-      <c r="A65" s="91"/>
+    <row r="65" spans="1:3" ht="15.6">
+      <c r="A65" s="108"/>
       <c r="B65" s="25" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15.6">
+      <c r="A66" s="108"/>
+      <c r="B66" s="25" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="16.399999999999999">
-      <c r="A66" s="91"/>
-      <c r="B66" s="25" t="s">
+    <row r="67" spans="1:3" ht="15.6">
+      <c r="A67" s="108"/>
+      <c r="B67" s="25" t="s">
         <v>193</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="16.399999999999999">
-      <c r="A67" s="91"/>
-      <c r="B67" s="25" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -3677,66 +3794,66 @@
       <c r="A69" s="16"/>
       <c r="B69" s="16"/>
     </row>
-    <row r="70" spans="1:3" ht="17.05">
+    <row r="70" spans="1:3" ht="16.2">
       <c r="A70" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B70" s="19" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="17.05">
+    <row r="71" spans="1:3" ht="16.2">
       <c r="A71" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="17.05">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="16.2">
       <c r="A72" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B72" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="16.399999999999999">
-      <c r="A73" s="90" t="s">
+    <row r="73" spans="1:3" ht="15.6">
+      <c r="A73" s="107" t="s">
         <v>36</v>
       </c>
       <c r="B73" s="25" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="16.399999999999999">
-      <c r="A74" s="91"/>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15.6">
+      <c r="A74" s="108"/>
       <c r="B74" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="16.399999999999999">
-      <c r="A75" s="91"/>
+    <row r="75" spans="1:3" ht="15.6">
+      <c r="A75" s="108"/>
       <c r="B75" s="25" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="15.6">
+      <c r="A76" s="108"/>
+      <c r="B76" s="25" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="16.399999999999999">
-      <c r="A76" s="91"/>
-      <c r="B76" s="25" t="s">
+    <row r="77" spans="1:3" ht="15.6">
+      <c r="A77" s="108"/>
+      <c r="B77" s="25" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="16.399999999999999">
-      <c r="A77" s="91"/>
-      <c r="B77" s="25" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -3747,93 +3864,93 @@
       <c r="A79" s="16"/>
       <c r="B79" s="16"/>
     </row>
-    <row r="80" spans="1:3" ht="17.05">
+    <row r="80" spans="1:3" ht="16.2">
       <c r="A80" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B80" s="19" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="17.05">
+    <row r="81" spans="1:3" ht="16.2">
       <c r="A81" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="16.399999999999999">
-      <c r="A82" s="92" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15.6">
+      <c r="A82" s="109" t="s">
         <v>34</v>
       </c>
       <c r="B82" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15.6">
+      <c r="A83" s="109"/>
+      <c r="B83" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15.6">
+      <c r="A84" s="109"/>
+      <c r="B84" s="24" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15.6">
+      <c r="A85" s="107" t="s">
+        <v>36</v>
+      </c>
+      <c r="B85" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="16.399999999999999">
-      <c r="A83" s="92"/>
-      <c r="B83" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="16.399999999999999">
-      <c r="A84" s="92"/>
-      <c r="B84" s="24" t="s">
+      <c r="C85" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="15.6">
+      <c r="A86" s="108"/>
+      <c r="B86" s="25" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="16.399999999999999">
-      <c r="A85" s="90" t="s">
-        <v>36</v>
-      </c>
-      <c r="B85" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="16.399999999999999">
-      <c r="A86" s="91"/>
-      <c r="B86" s="25" t="s">
+    <row r="87" spans="1:3" ht="15.6">
+      <c r="A87" s="108"/>
+      <c r="B87" s="25" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="16.399999999999999">
-      <c r="A87" s="91"/>
-      <c r="B87" s="25" t="s">
+    <row r="88" spans="1:3" ht="15.6">
+      <c r="A88" s="108"/>
+      <c r="B88" s="25" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="16.399999999999999">
-      <c r="A88" s="91"/>
-      <c r="B88" s="25" t="s">
+    <row r="89" spans="1:3" ht="15.6">
+      <c r="A89" s="108"/>
+      <c r="B89" s="25" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="16.399999999999999">
-      <c r="A89" s="91"/>
-      <c r="B89" s="25" t="s">
+    <row r="90" spans="1:3" ht="15.6">
+      <c r="A90" s="108"/>
+      <c r="B90" s="25" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="16.399999999999999">
-      <c r="A90" s="91"/>
-      <c r="B90" s="25" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="16.399999999999999">
-      <c r="A91" s="91"/>
+    <row r="91" spans="1:3" ht="15.6">
+      <c r="A91" s="108"/>
       <c r="B91" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -3844,72 +3961,72 @@
       <c r="A93" s="16"/>
       <c r="B93" s="16"/>
     </row>
-    <row r="94" spans="1:3" ht="17.05">
+    <row r="94" spans="1:3" ht="16.2">
       <c r="A94" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="B94" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="16.2">
+      <c r="A95" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="15.6">
+      <c r="A96" s="109" t="s">
+        <v>34</v>
+      </c>
+      <c r="B96" s="24" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="15.6">
+      <c r="A97" s="109"/>
+      <c r="B97" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="B94" s="19" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="17.05">
-      <c r="A95" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="B95" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="16.399999999999999">
-      <c r="A96" s="92" t="s">
-        <v>34</v>
-      </c>
-      <c r="B96" s="24" t="s">
+    </row>
+    <row r="98" spans="1:6" ht="15.6">
+      <c r="A98" s="109"/>
+      <c r="B98" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="15.6">
+      <c r="A99" s="109"/>
+      <c r="B99" s="24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="15.6">
+      <c r="A100" s="109"/>
+      <c r="B100" s="24" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="15.6">
+      <c r="A101" s="107" t="s">
+        <v>36</v>
+      </c>
+      <c r="B101" s="25" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" ht="16.399999999999999">
-      <c r="A97" s="92"/>
-      <c r="B97" s="24" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="16.399999999999999">
-      <c r="A98" s="92"/>
-      <c r="B98" s="24" t="s">
-        <v>211</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="16.399999999999999">
-      <c r="A99" s="92"/>
-      <c r="B99" s="24" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="16.399999999999999">
-      <c r="A100" s="92"/>
-      <c r="B100" s="24" t="s">
+      <c r="C101" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="15.6">
+      <c r="A102" s="108"/>
+      <c r="B102" s="25" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="16.399999999999999">
-      <c r="A101" s="90" t="s">
-        <v>36</v>
-      </c>
-      <c r="B101" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="16.399999999999999">
-      <c r="A102" s="91"/>
-      <c r="B102" s="25" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -3920,479 +4037,474 @@
       <c r="A104" s="12"/>
       <c r="B104" s="12"/>
     </row>
-    <row r="105" spans="1:6" ht="17.05">
+    <row r="105" spans="1:6" ht="16.2">
       <c r="A105" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B105" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="16.2">
+      <c r="A106" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B106" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B105" s="19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="17.05">
-      <c r="A106" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="B106" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="C106" s="1" t="s">
+    </row>
+    <row r="107" spans="1:6" ht="15.6">
+      <c r="A107" s="109" t="s">
+        <v>34</v>
+      </c>
+      <c r="B107" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="15.6">
+      <c r="A108" s="109"/>
+      <c r="B108" s="24" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="16.399999999999999">
-      <c r="A107" s="92" t="s">
-        <v>34</v>
-      </c>
-      <c r="B107" s="24" t="s">
-        <v>187</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" ht="16.399999999999999">
-      <c r="A108" s="92"/>
-      <c r="B108" s="24" t="s">
+    <row r="109" spans="1:6" ht="15.6">
+      <c r="A109" s="107" t="s">
+        <v>36</v>
+      </c>
+      <c r="B109" s="25" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" ht="16.399999999999999">
-      <c r="A109" s="90" t="s">
-        <v>36</v>
-      </c>
-      <c r="B109" s="25" t="s">
+      <c r="C109" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="15.6">
+      <c r="A110" s="108"/>
+      <c r="B110" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" ht="16.399999999999999">
-      <c r="A110" s="91"/>
-      <c r="B110" s="25" t="s">
+      <c r="C110" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="15">
+      <c r="A111" s="108"/>
+      <c r="B111" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6">
-      <c r="A111" s="91"/>
-      <c r="B111" s="28" t="s">
+      <c r="C111" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C111" s="1" t="s">
+    </row>
+    <row r="112" spans="1:6" ht="15.6">
+      <c r="A112" s="108"/>
+      <c r="B112" s="25" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" ht="16.399999999999999">
-      <c r="A112" s="91"/>
-      <c r="B112" s="25" t="s">
+      <c r="C112" s="94" t="s">
         <v>222</v>
       </c>
-      <c r="C112" s="99" t="s">
-        <v>223</v>
-      </c>
-      <c r="D112" s="99"/>
-      <c r="E112" s="99"/>
-      <c r="F112" s="99"/>
+      <c r="D112" s="94"/>
+      <c r="E112" s="94"/>
+      <c r="F112" s="94"/>
     </row>
     <row r="113" spans="1:6" ht="162" customHeight="1">
       <c r="A113" s="12"/>
       <c r="B113" s="12"/>
-      <c r="C113" s="99"/>
-      <c r="D113" s="99"/>
-      <c r="E113" s="99"/>
-      <c r="F113" s="99"/>
-    </row>
-    <row r="117" spans="1:6" ht="17.05">
+      <c r="C113" s="94"/>
+      <c r="D113" s="94"/>
+      <c r="E113" s="94"/>
+      <c r="F113" s="94"/>
+    </row>
+    <row r="117" spans="1:6" ht="16.2">
       <c r="A117" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B117" s="19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" ht="17.05">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="16.2">
       <c r="A118" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" ht="17.05">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="16.2">
       <c r="A119" s="29" t="s">
         <v>34</v>
       </c>
       <c r="B119" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="15.6">
+      <c r="A120" s="107" t="s">
+        <v>36</v>
+      </c>
+      <c r="B120" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" ht="16.399999999999999">
-      <c r="A120" s="90" t="s">
-        <v>36</v>
-      </c>
-      <c r="B120" s="26" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" ht="16.399999999999999">
-      <c r="A121" s="91"/>
+    </row>
+    <row r="121" spans="1:6" ht="15.6">
+      <c r="A121" s="108"/>
       <c r="B121" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="15.6">
+      <c r="A122" s="108"/>
+      <c r="B122" s="26" t="s">
         <v>225</v>
       </c>
-      <c r="C121" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" ht="16.399999999999999">
-      <c r="A122" s="91"/>
-      <c r="B122" s="26" t="s">
+    </row>
+    <row r="123" spans="1:6" ht="15.6">
+      <c r="A123" s="108"/>
+      <c r="B123" s="26" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="16.399999999999999">
-      <c r="A123" s="91"/>
-      <c r="B123" s="26" t="s">
+    <row r="124" spans="1:6" ht="15.6">
+      <c r="A124" s="108"/>
+      <c r="B124" s="26" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="16.399999999999999">
-      <c r="A124" s="91"/>
-      <c r="B124" s="26" t="s">
+    <row r="125" spans="1:6" ht="15.6">
+      <c r="A125" s="108"/>
+      <c r="B125" s="26" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="16.399999999999999">
-      <c r="A125" s="91"/>
-      <c r="B125" s="26" t="s">
+    <row r="126" spans="1:6" ht="15.6">
+      <c r="A126" s="108"/>
+      <c r="B126" s="26" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="16.399999999999999">
-      <c r="A126" s="91"/>
-      <c r="B126" s="26" t="s">
+    <row r="129" spans="1:12" ht="16.2">
+      <c r="A129" s="106" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="129" spans="1:12" ht="17.05">
-      <c r="A129" s="88" t="s">
+      <c r="B129" s="106"/>
+    </row>
+    <row r="130" spans="1:12" ht="16.2">
+      <c r="A130" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="B129" s="88"/>
-    </row>
-    <row r="130" spans="1:12" ht="17.05">
-      <c r="A130" s="19" t="s">
-        <v>232</v>
-      </c>
       <c r="B130" s="19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="131" spans="1:12" ht="17.05">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" ht="16.2">
       <c r="A131" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B131" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="132" spans="1:12" ht="17.05">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" ht="16.2">
       <c r="A132" s="29" t="s">
         <v>34</v>
       </c>
       <c r="B132" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" ht="15.6">
+      <c r="A133" s="87" t="s">
+        <v>36</v>
+      </c>
+      <c r="B133" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="C132" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="133" spans="1:12" ht="16.399999999999999">
-      <c r="A133" s="93" t="s">
-        <v>36</v>
-      </c>
-      <c r="B133" s="24" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="134" spans="1:12" ht="16.399999999999999">
-      <c r="A134" s="94"/>
+    </row>
+    <row r="134" spans="1:12" ht="15.6">
+      <c r="A134" s="88"/>
       <c r="B134" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" ht="15.6">
+      <c r="A135" s="88"/>
+      <c r="B135" s="26" t="s">
         <v>233</v>
       </c>
-      <c r="C134" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="135" spans="1:12" ht="16.399999999999999">
-      <c r="A135" s="94"/>
-      <c r="B135" s="26" t="s">
+    </row>
+    <row r="136" spans="1:12" ht="15.6">
+      <c r="A136" s="88"/>
+      <c r="B136" s="26" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="136" spans="1:12" ht="16.399999999999999">
-      <c r="A136" s="94"/>
-      <c r="B136" s="26" t="s">
+    <row r="137" spans="1:12" ht="15.6">
+      <c r="A137" s="88"/>
+      <c r="B137" s="26" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="137" spans="1:12" ht="16.399999999999999">
-      <c r="A137" s="94"/>
-      <c r="B137" s="26" t="s">
+    <row r="138" spans="1:12" ht="15.6">
+      <c r="A138" s="89"/>
+      <c r="B138" s="26" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="138" spans="1:12" ht="16.399999999999999">
-      <c r="A138" s="95"/>
-      <c r="B138" s="26" t="s">
+    <row r="140" spans="1:12">
+      <c r="A140" s="90" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="140" spans="1:12">
-      <c r="A140" s="89" t="s">
+      <c r="B140" s="95" t="s">
         <v>238</v>
       </c>
-      <c r="B140" s="100" t="s">
+      <c r="C140" s="96"/>
+      <c r="D140" s="96"/>
+      <c r="E140" s="96"/>
+      <c r="F140" s="96"/>
+      <c r="G140" s="96"/>
+      <c r="H140" s="96"/>
+      <c r="I140" s="96"/>
+      <c r="J140" s="96"/>
+      <c r="K140" s="96"/>
+      <c r="L140" s="97"/>
+    </row>
+    <row r="141" spans="1:12">
+      <c r="A141" s="91"/>
+      <c r="B141" s="98"/>
+      <c r="C141" s="99"/>
+      <c r="D141" s="99"/>
+      <c r="E141" s="99"/>
+      <c r="F141" s="99"/>
+      <c r="G141" s="99"/>
+      <c r="H141" s="99"/>
+      <c r="I141" s="99"/>
+      <c r="J141" s="99"/>
+      <c r="K141" s="99"/>
+      <c r="L141" s="100"/>
+    </row>
+    <row r="142" spans="1:12">
+      <c r="A142" s="91"/>
+      <c r="B142" s="98"/>
+      <c r="C142" s="99"/>
+      <c r="D142" s="99"/>
+      <c r="E142" s="99"/>
+      <c r="F142" s="99"/>
+      <c r="G142" s="99"/>
+      <c r="H142" s="99"/>
+      <c r="I142" s="99"/>
+      <c r="J142" s="99"/>
+      <c r="K142" s="99"/>
+      <c r="L142" s="100"/>
+    </row>
+    <row r="143" spans="1:12">
+      <c r="A143" s="91"/>
+      <c r="B143" s="98"/>
+      <c r="C143" s="99"/>
+      <c r="D143" s="99"/>
+      <c r="E143" s="99"/>
+      <c r="F143" s="99"/>
+      <c r="G143" s="99"/>
+      <c r="H143" s="99"/>
+      <c r="I143" s="99"/>
+      <c r="J143" s="99"/>
+      <c r="K143" s="99"/>
+      <c r="L143" s="100"/>
+    </row>
+    <row r="144" spans="1:12">
+      <c r="A144" s="91"/>
+      <c r="B144" s="98"/>
+      <c r="C144" s="99"/>
+      <c r="D144" s="99"/>
+      <c r="E144" s="99"/>
+      <c r="F144" s="99"/>
+      <c r="G144" s="99"/>
+      <c r="H144" s="99"/>
+      <c r="I144" s="99"/>
+      <c r="J144" s="99"/>
+      <c r="K144" s="99"/>
+      <c r="L144" s="100"/>
+    </row>
+    <row r="145" spans="1:12">
+      <c r="A145" s="91"/>
+      <c r="B145" s="98"/>
+      <c r="C145" s="99"/>
+      <c r="D145" s="99"/>
+      <c r="E145" s="99"/>
+      <c r="F145" s="99"/>
+      <c r="G145" s="99"/>
+      <c r="H145" s="99"/>
+      <c r="I145" s="99"/>
+      <c r="J145" s="99"/>
+      <c r="K145" s="99"/>
+      <c r="L145" s="100"/>
+    </row>
+    <row r="146" spans="1:12" ht="25.05" customHeight="1">
+      <c r="A146" s="91"/>
+      <c r="B146" s="101"/>
+      <c r="C146" s="102"/>
+      <c r="D146" s="102"/>
+      <c r="E146" s="102"/>
+      <c r="F146" s="102"/>
+      <c r="G146" s="102"/>
+      <c r="H146" s="102"/>
+      <c r="I146" s="102"/>
+      <c r="J146" s="102"/>
+      <c r="K146" s="102"/>
+      <c r="L146" s="103"/>
+    </row>
+    <row r="150" spans="1:12" ht="16.2">
+      <c r="A150" s="30" t="s">
         <v>239</v>
       </c>
-      <c r="C140" s="101"/>
-      <c r="D140" s="101"/>
-      <c r="E140" s="101"/>
-      <c r="F140" s="101"/>
-      <c r="G140" s="101"/>
-      <c r="H140" s="101"/>
-      <c r="I140" s="101"/>
-      <c r="J140" s="101"/>
-      <c r="K140" s="101"/>
-      <c r="L140" s="102"/>
-    </row>
-    <row r="141" spans="1:12">
-      <c r="A141" s="96"/>
-      <c r="B141" s="103"/>
-      <c r="C141" s="104"/>
-      <c r="D141" s="104"/>
-      <c r="E141" s="104"/>
-      <c r="F141" s="104"/>
-      <c r="G141" s="104"/>
-      <c r="H141" s="104"/>
-      <c r="I141" s="104"/>
-      <c r="J141" s="104"/>
-      <c r="K141" s="104"/>
-      <c r="L141" s="105"/>
-    </row>
-    <row r="142" spans="1:12">
-      <c r="A142" s="96"/>
-      <c r="B142" s="103"/>
-      <c r="C142" s="104"/>
-      <c r="D142" s="104"/>
-      <c r="E142" s="104"/>
-      <c r="F142" s="104"/>
-      <c r="G142" s="104"/>
-      <c r="H142" s="104"/>
-      <c r="I142" s="104"/>
-      <c r="J142" s="104"/>
-      <c r="K142" s="104"/>
-      <c r="L142" s="105"/>
-    </row>
-    <row r="143" spans="1:12">
-      <c r="A143" s="96"/>
-      <c r="B143" s="103"/>
-      <c r="C143" s="104"/>
-      <c r="D143" s="104"/>
-      <c r="E143" s="104"/>
-      <c r="F143" s="104"/>
-      <c r="G143" s="104"/>
-      <c r="H143" s="104"/>
-      <c r="I143" s="104"/>
-      <c r="J143" s="104"/>
-      <c r="K143" s="104"/>
-      <c r="L143" s="105"/>
-    </row>
-    <row r="144" spans="1:12">
-      <c r="A144" s="96"/>
-      <c r="B144" s="103"/>
-      <c r="C144" s="104"/>
-      <c r="D144" s="104"/>
-      <c r="E144" s="104"/>
-      <c r="F144" s="104"/>
-      <c r="G144" s="104"/>
-      <c r="H144" s="104"/>
-      <c r="I144" s="104"/>
-      <c r="J144" s="104"/>
-      <c r="K144" s="104"/>
-      <c r="L144" s="105"/>
-    </row>
-    <row r="145" spans="1:12">
-      <c r="A145" s="96"/>
-      <c r="B145" s="103"/>
-      <c r="C145" s="104"/>
-      <c r="D145" s="104"/>
-      <c r="E145" s="104"/>
-      <c r="F145" s="104"/>
-      <c r="G145" s="104"/>
-      <c r="H145" s="104"/>
-      <c r="I145" s="104"/>
-      <c r="J145" s="104"/>
-      <c r="K145" s="104"/>
-      <c r="L145" s="105"/>
-    </row>
-    <row r="146" spans="1:12" ht="25.05" customHeight="1">
-      <c r="A146" s="96"/>
-      <c r="B146" s="106"/>
-      <c r="C146" s="107"/>
-      <c r="D146" s="107"/>
-      <c r="E146" s="107"/>
-      <c r="F146" s="107"/>
-      <c r="G146" s="107"/>
-      <c r="H146" s="107"/>
-      <c r="I146" s="107"/>
-      <c r="J146" s="107"/>
-      <c r="K146" s="107"/>
-      <c r="L146" s="108"/>
-    </row>
-    <row r="150" spans="1:12" ht="17.05">
-      <c r="A150" s="30" t="s">
-        <v>240</v>
-      </c>
       <c r="B150" s="31" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="151" spans="1:12" ht="17.05">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" ht="16.2">
       <c r="A151" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B151" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="152" spans="1:12" ht="17.05">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" ht="16.2">
       <c r="A152" s="29" t="s">
         <v>34</v>
       </c>
       <c r="B152" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" ht="15.6">
+      <c r="A153" s="92" t="s">
+        <v>36</v>
+      </c>
+      <c r="B153" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="C152" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="153" spans="1:12" ht="16.399999999999999">
-      <c r="A153" s="97" t="s">
-        <v>36</v>
-      </c>
-      <c r="B153" s="26" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="154" spans="1:12" ht="16.399999999999999">
-      <c r="A154" s="98"/>
+    </row>
+    <row r="154" spans="1:12" ht="15.6">
+      <c r="A154" s="93"/>
       <c r="B154" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" ht="15.6">
+      <c r="A155" s="93"/>
+      <c r="B155" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="C154" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="155" spans="1:12" ht="16.399999999999999">
-      <c r="A155" s="98"/>
-      <c r="B155" s="26" t="s">
+    </row>
+    <row r="156" spans="1:12" ht="15.6">
+      <c r="A156" s="93"/>
+      <c r="B156" s="26" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="156" spans="1:12" ht="16.399999999999999">
-      <c r="A156" s="98"/>
-      <c r="B156" s="26" t="s">
+    <row r="157" spans="1:12" ht="15.6">
+      <c r="A157" s="93"/>
+      <c r="B157" s="26" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="157" spans="1:12" ht="16.399999999999999">
-      <c r="A157" s="98"/>
-      <c r="B157" s="26" t="s">
+    <row r="158" spans="1:12" ht="15.6">
+      <c r="A158" s="93"/>
+      <c r="B158" s="26" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="158" spans="1:12" ht="16.399999999999999">
-      <c r="A158" s="98"/>
-      <c r="B158" s="26" t="s">
+    <row r="159" spans="1:12" ht="15.6">
+      <c r="A159" s="93"/>
+      <c r="B159" s="26" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="159" spans="1:12" ht="16.399999999999999">
-      <c r="A159" s="98"/>
-      <c r="B159" s="26" t="s">
+    <row r="160" spans="1:12" ht="15.6">
+      <c r="A160" s="93"/>
+      <c r="B160" s="26" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="160" spans="1:12" ht="16.399999999999999">
-      <c r="A160" s="98"/>
-      <c r="B160" s="26" t="s">
+      <c r="C160" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C160" s="1" t="s">
+    </row>
+    <row r="161" spans="1:3" ht="15.6">
+      <c r="A161" s="93"/>
+      <c r="B161" s="26" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" ht="16.399999999999999">
-      <c r="A161" s="98"/>
-      <c r="B161" s="26" t="s">
+      <c r="C161" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="15.6">
+      <c r="A162" s="93"/>
+      <c r="B162" s="26" t="s">
         <v>249</v>
       </c>
-      <c r="C161" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="16.399999999999999">
-      <c r="A162" s="98"/>
-      <c r="B162" s="26" t="s">
+    </row>
+    <row r="163" spans="1:3" ht="15.6">
+      <c r="A163" s="93"/>
+      <c r="B163" s="26" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="16.399999999999999">
-      <c r="A163" s="98"/>
-      <c r="B163" s="26" t="s">
+    <row r="164" spans="1:3" ht="15.6">
+      <c r="A164" s="93"/>
+      <c r="B164" s="26" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="16.399999999999999">
-      <c r="A164" s="98"/>
-      <c r="B164" s="26" t="s">
+    <row r="165" spans="1:3" ht="15.6">
+      <c r="A165" s="93"/>
+      <c r="B165" s="26" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="16.399999999999999">
-      <c r="A165" s="98"/>
-      <c r="B165" s="26" t="s">
+    <row r="166" spans="1:3" ht="15.6">
+      <c r="A166" s="93"/>
+      <c r="B166" s="26" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" ht="16.399999999999999">
-      <c r="A166" s="98"/>
-      <c r="B166" s="26" t="s">
+      <c r="C166" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C166" s="1" t="s">
+    </row>
+    <row r="167" spans="1:3" ht="15.6">
+      <c r="A167" s="93"/>
+      <c r="B167" s="26" t="s">
         <v>255</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" ht="16.399999999999999">
-      <c r="A167" s="98"/>
-      <c r="B167" s="26" t="s">
-        <v>256</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A133:A138"/>
-    <mergeCell ref="A140:A146"/>
-    <mergeCell ref="A153:A167"/>
-    <mergeCell ref="C112:F113"/>
-    <mergeCell ref="B140:L146"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="C57:D57"/>
@@ -4408,6 +4520,11 @@
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="A109:A112"/>
     <mergeCell ref="A120:A126"/>
+    <mergeCell ref="A133:A138"/>
+    <mergeCell ref="A140:A146"/>
+    <mergeCell ref="A153:A167"/>
+    <mergeCell ref="C112:F113"/>
+    <mergeCell ref="B140:L146"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>